<commit_message>
update logs and proposal
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\MDS\capstone\w2020-data599-capstone-projects-ubc-udl\personal-logs\nathan-smith\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90792D2-6BBC-44D9-84BD-B5A1607382AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE7C53C-9202-4291-98F7-40B7C42B47D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -132,6 +132,51 @@
   </si>
   <si>
     <t>Nathan Smith</t>
+  </si>
+  <si>
+    <t>Discuss Gantt chart and tasks</t>
+  </si>
+  <si>
+    <t>Update Gantt chart and upload to OneDrive for client</t>
+  </si>
+  <si>
+    <t>Stand-up</t>
+  </si>
+  <si>
+    <t>Work on proposal/review progress to date on it</t>
+  </si>
+  <si>
+    <t>Meeting with client to discuss project</t>
+  </si>
+  <si>
+    <t>Internal post client meeting</t>
+  </si>
+  <si>
+    <t>Update meeting minutes</t>
+  </si>
+  <si>
+    <t>Update Gantt chart</t>
+  </si>
+  <si>
+    <t>Work on proposal statement of work section</t>
+  </si>
+  <si>
+    <t>Work on proposal</t>
+  </si>
+  <si>
+    <t>Scrum meeting with client</t>
+  </si>
+  <si>
+    <t>Kanban board organization and scrum meeting document clean-up</t>
+  </si>
+  <si>
+    <t>Finish draft proposal</t>
+  </si>
+  <si>
+    <t>Update proposal with client comments</t>
+  </si>
+  <si>
+    <t>Proposal Presentation</t>
   </si>
 </sst>
 </file>
@@ -735,7 +780,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -840,6 +885,12 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="20" borderId="19" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -848,11 +899,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="20" borderId="19" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -900,126 +946,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -1615,8 +1542,8 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -1711,12 +1638,12 @@
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="31">
+      <c r="A14" s="34">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
@@ -1827,12 +1754,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="31">
+      <c r="A25" s="34">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
@@ -1923,9 +1850,15 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="20"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="27">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="20"/>
@@ -1933,56 +1866,106 @@
       <c r="C35" s="27"/>
       <c r="D35">
         <f>SUM(C26:C35)</f>
-        <v>7.25</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="31">
+      <c r="A36" s="34">
         <f>A25+1</f>
         <v>44321</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="33"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="18"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="18"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="18"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+      <c r="A41" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="33"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="18"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="19"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="D43" s="33"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="20"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="27">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="20"/>
@@ -1995,46 +1978,82 @@
       <c r="C46" s="27"/>
       <c r="D46">
         <f>SUM(C37:C46)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="31">
+      <c r="A47" s="34">
         <f>A36+1</f>
         <v>44322</v>
       </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="33"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="31"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="18"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
+      <c r="A48" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="18"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="A49" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="25">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="18"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="18"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="25">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="19"/>
@@ -2057,31 +2076,49 @@
       <c r="C57" s="27"/>
       <c r="D57">
         <f>SUM(C48:C57)</f>
-        <v>0</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="31">
+      <c r="A58" s="34">
         <f>A47+1</f>
         <v>44323</v>
       </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="33"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="31"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="18"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="25">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="18"/>
@@ -2119,16 +2156,16 @@
       <c r="C68" s="27"/>
       <c r="D68">
         <f>SUM(C59:C68)</f>
-        <v>0</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="31">
+      <c r="A69" s="34">
         <f>A58+1</f>
         <v>44324</v>
       </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="33"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="31"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="18"/>
@@ -2185,12 +2222,12 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="31">
+      <c r="A80" s="34">
         <f>A69+1</f>
         <v>44325</v>
       </c>
-      <c r="B80" s="32"/>
-      <c r="C80" s="33"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="31"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="18"/>
@@ -2262,9 +2299,9 @@
         <v>5</v>
       </c>
       <c r="B93" s="17"/>
-      <c r="C93" s="34">
+      <c r="C93" s="32">
         <f>SUM(C14:C90)</f>
-        <v>17.5</v>
+        <v>36.5</v>
       </c>
       <c r="D93" s="13"/>
     </row>
@@ -2308,156 +2345,156 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="47" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="46" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="44" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="43" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="41" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="40" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="39" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="38" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="37" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="36" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="32" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="27" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="22" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="19" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update proposal and meeting minutes
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE7C53C-9202-4291-98F7-40B7C42B47D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0FD9BF-204F-4151-84F4-2CDA7FB98B60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>Proposal Presentation</t>
+  </si>
+  <si>
+    <t>High-level review of anomaly detection algorithms</t>
+  </si>
+  <si>
+    <t>Finalize proposal and presentation</t>
+  </si>
+  <si>
+    <t>Update GitHub READMEs</t>
   </si>
 </sst>
 </file>
@@ -1542,8 +1551,8 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -2117,13 +2126,19 @@
         <v>24</v>
       </c>
       <c r="C61" s="25">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="18"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
+      <c r="A62" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="18"/>
@@ -2156,7 +2171,7 @@
       <c r="C68" s="27"/>
       <c r="D68">
         <f>SUM(C59:C68)</f>
-        <v>5.25</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2168,14 +2183,26 @@
       <c r="C69" s="31"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="18"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
+      <c r="A70" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
+      <c r="A71" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="18"/>
@@ -2218,7 +2245,7 @@
       <c r="C79" s="27"/>
       <c r="D79">
         <f>SUM(C70:C79)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2301,7 +2328,7 @@
       <c r="B93" s="17"/>
       <c r="C93" s="32">
         <f>SUM(C14:C90)</f>
-        <v>36.5</v>
+        <v>38.5</v>
       </c>
       <c r="D93" s="13"/>
     </row>

</xml_diff>

<commit_message>
update logs and presentation
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707D161C-0A4E-460D-9B7A-DEBE189E6669}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94190982-F25D-488C-BD6F-131D29297007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>Parsing Files</t>
+  </si>
+  <si>
+    <t>Logs and GitHub cleanup</t>
+  </si>
+  <si>
+    <t>Research how streaming anomaly detection would wrok with InfluxDB</t>
+  </si>
+  <si>
+    <t>InfluxDB Streaming</t>
+  </si>
+  <si>
+    <t>Stand-up and presentation run-through</t>
   </si>
 </sst>
 </file>
@@ -2796,7 +2808,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -3003,24 +3015,48 @@
       <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="18"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="25">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="18"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="18"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
@@ -3053,7 +3089,7 @@
       <c r="C35" s="27"/>
       <c r="D35">
         <f>SUM(C26:C35)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3386,7 +3422,7 @@
       <c r="B93" s="17"/>
       <c r="C93" s="32">
         <f>SUM(C14:C90)</f>
-        <v>11</v>
+        <v>13.5</v>
       </c>
       <c r="D93" s="13"/>
     </row>
@@ -3444,152 +3480,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="27" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="25" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="23" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="22" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="21" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="20" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="18" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add weekly update and logs
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94190982-F25D-488C-BD6F-131D29297007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0BF211-1C71-42E2-9A4C-BB7AF3C06B39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$D$68</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$D$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$D$69</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -220,13 +220,94 @@
     <t>Logs and GitHub cleanup</t>
   </si>
   <si>
-    <t>Research how streaming anomaly detection would wrok with InfluxDB</t>
-  </si>
-  <si>
     <t>InfluxDB Streaming</t>
   </si>
   <si>
     <t>Stand-up and presentation run-through</t>
+  </si>
+  <si>
+    <t>Research how streaming anomaly detection would work with InfluxDB</t>
+  </si>
+  <si>
+    <t>Presentation (incl prep before)</t>
+  </si>
+  <si>
+    <t>Figure out and code a simple simulator in Python not reliant on InfluxDB</t>
+  </si>
+  <si>
+    <t>Streaming Simulation</t>
+  </si>
+  <si>
+    <t>Project file clean-up</t>
+  </si>
+  <si>
+    <t>Testing using telegraf reading data from InfluxDB</t>
+  </si>
+  <si>
+    <t>Extended stand-up to discuss where we're each at</t>
+  </si>
+  <si>
+    <t>Meeting with Ryan to discuss data parsing</t>
+  </si>
+  <si>
+    <t>Data parsing</t>
+  </si>
+  <si>
+    <t>Influxdb streaming and parsing</t>
+  </si>
+  <si>
+    <t>Data parsing and streaming</t>
+  </si>
+  <si>
+    <t>Setup sprint planning doc</t>
+  </si>
+  <si>
+    <t>Clean-up streaming research and PR files and discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand-up and sprint planning discussion </t>
+  </si>
+  <si>
+    <t>Parsing discussions/research</t>
+  </si>
+  <si>
+    <t>InfluxDB Parsing</t>
+  </si>
+  <si>
+    <t>Kanban board updates</t>
+  </si>
+  <si>
+    <t>Streaming system ppt slides for meeting</t>
+  </si>
+  <si>
+    <t>Sprint planning meeting</t>
+  </si>
+  <si>
+    <t>Meeting with client</t>
+  </si>
+  <si>
+    <t>Post-sprint meeting</t>
+  </si>
+  <si>
+    <t>Clean-up meeting minutes and streaming ppt for Jiachen to talk to EWS</t>
+  </si>
+  <si>
+    <t>Testing various InfluxDB streaming methods</t>
+  </si>
+  <si>
+    <t>Streaming parsing work</t>
+  </si>
+  <si>
+    <t>Dealing with python environment issues</t>
+  </si>
+  <si>
+    <t>IncluxDB Streaming</t>
+  </si>
+  <si>
+    <t>Work on weekly presentation</t>
+  </si>
+  <si>
+    <t>Upload OneDrive documents to GitHub with updated logs</t>
   </si>
 </sst>
 </file>
@@ -530,7 +611,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -783,6 +864,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -830,7 +939,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -941,6 +1050,14 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="20" borderId="19" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -996,7 +1113,210 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="91">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1809,7 +2129,7 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
@@ -1905,11 +2225,11 @@
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="34">
+      <c r="A14" s="36">
         <f>D3</f>
         <v>44319</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -2021,11 +2341,11 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="34">
+      <c r="A25" s="36">
         <f>A14+1</f>
         <v>44320</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -2137,11 +2457,11 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="34">
+      <c r="A36" s="36">
         <f>A25+1</f>
         <v>44321</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -2249,11 +2569,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="34">
+      <c r="A47" s="36">
         <f>A36+1</f>
         <v>44322</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="31"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -2347,11 +2667,11 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="34">
+      <c r="A58" s="36">
         <f>A47+1</f>
         <v>44323</v>
       </c>
-      <c r="B58" s="35"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="31"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -2433,11 +2753,11 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="34">
+      <c r="A69" s="36">
         <f>A58+1</f>
         <v>44324</v>
       </c>
-      <c r="B69" s="35"/>
+      <c r="B69" s="37"/>
       <c r="C69" s="31"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -2507,11 +2827,11 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="34">
+      <c r="A80" s="36">
         <f>A69+1</f>
         <v>44325</v>
       </c>
-      <c r="B80" s="35"/>
+      <c r="B80" s="37"/>
       <c r="C80" s="31"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -2639,157 +2959,157 @@
     <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="61" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="60" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="59" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="58" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="57" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="56" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="55" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="54" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="53" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="52" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="51" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="50" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="49" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="48" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="47" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="46" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="45" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="44" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="43" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="42" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="41" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="40" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="39" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="38" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="37" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="36" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="34" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="32" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="31" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2805,10 +3125,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -2903,11 +3223,11 @@
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="34">
+      <c r="A14" s="36">
         <f>D3</f>
         <v>44326</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -3007,11 +3327,11 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="34">
+      <c r="A25" s="36">
         <f>A14+1</f>
         <v>44327</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -3038,10 +3358,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>65</v>
       </c>
       <c r="C28" s="25">
         <v>0.25</v>
@@ -3049,7 +3369,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>21</v>
@@ -3059,19 +3379,37 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="18"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="19"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
+      <c r="A32" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="26">
+        <v>4.25</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="20"/>
@@ -3089,47 +3427,83 @@
       <c r="C35" s="27"/>
       <c r="D35">
         <f>SUM(C26:C35)</f>
-        <v>2.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="34">
+      <c r="A36" s="36">
         <f>A25+1</f>
         <v>44328</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="25">
+        <v>2.75</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="18"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="18"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="18"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+      <c r="A41" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="25">
+        <v>2</v>
+      </c>
       <c r="D41" s="33"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="18"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="19"/>
@@ -3153,145 +3527,253 @@
       <c r="C46" s="27"/>
       <c r="D46">
         <f>SUM(C37:C46)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="34">
+      <c r="A47" s="36">
         <f>A36+1</f>
         <v>44329</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="31"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="18"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
+      <c r="A48" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="25">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="18"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="A49" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="18"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="18"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="19"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
+      <c r="A54" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="26">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="20"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
+      <c r="A55" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" s="26">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="20"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="20"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57">
-        <f>SUM(C48:C57)</f>
-        <v>0</v>
+      <c r="A56" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="34">
+      <c r="A58" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="34">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <f>SUM(C48:C58)</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="36">
         <f>A47+1</f>
         <v>44330</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="31"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="18"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="31"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="25">
+        <v>3.25</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="18"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
+      <c r="A62" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="18"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
+      <c r="A63" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="18"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
+      <c r="A64" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="19"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
+      <c r="A65" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="25">
+        <v>2.75</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="20"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="26">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="20"/>
       <c r="B67" s="27"/>
       <c r="C67" s="27"/>
     </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="20"/>
       <c r="B68" s="27"/>
       <c r="C68" s="27"/>
-      <c r="D68">
-        <f>SUM(C59:C68)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="34">
-        <f>A58+1</f>
+      <c r="A69" s="20"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69">
+        <f>SUM(C60:C69)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="36">
+        <f>A59+1</f>
         <v>44331</v>
       </c>
-      <c r="B69" s="35"/>
-      <c r="C69" s="31"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" s="18"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="31"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="18"/>
@@ -3319,41 +3801,41 @@
       <c r="C75" s="25"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" s="19"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="26"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="20"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="27"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="20"/>
       <c r="B78" s="27"/>
       <c r="C78" s="27"/>
     </row>
-    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="20"/>
       <c r="B79" s="27"/>
       <c r="C79" s="27"/>
-      <c r="D79">
-        <f>SUM(C70:C79)</f>
+    </row>
+    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="20"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
+      <c r="D80">
+        <f>SUM(C71:C80)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="34">
-        <f>A69+1</f>
+    <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="36">
+        <f>A70+1</f>
         <v>44332</v>
       </c>
-      <c r="B80" s="35"/>
-      <c r="C80" s="31"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="18"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="31"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="18"/>
@@ -3381,14 +3863,14 @@
       <c r="C86" s="25"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" s="19"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
+      <c r="A87" s="18"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" s="20"/>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
+      <c r="A88" s="19"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="20"/>
@@ -3399,50 +3881,50 @@
       <c r="A90" s="20"/>
       <c r="B90" s="27"/>
       <c r="C90" s="27"/>
-      <c r="D90">
-        <f>SUM(C81:C90)</f>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="20"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91">
+        <f>SUM(C82:C91)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" s="21"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-    </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" s="10"/>
-      <c r="B92" s="28"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="12"/>
-    </row>
-    <row r="93" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="17" t="s">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="10"/>
+      <c r="B93" s="28"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="12"/>
+    </row>
+    <row r="94" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="17"/>
-      <c r="C93" s="32">
-        <f>SUM(C14:C90)</f>
-        <v>13.5</v>
-      </c>
-      <c r="D93" s="13"/>
-    </row>
-    <row r="94" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="9"/>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
-    </row>
-    <row r="95" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A95" s="10" t="s">
+      <c r="B94" s="17"/>
+      <c r="C94" s="32">
+        <f>SUM(C14:C91)</f>
+        <v>48</v>
+      </c>
+      <c r="D94" s="13"/>
+    </row>
+    <row r="95" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="9"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+    </row>
+    <row r="96" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A96" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="11"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="22"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="30"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="11"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="22"/>
@@ -3450,182 +3932,332 @@
       <c r="C97" s="30"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="9"/>
-      <c r="B98" s="29"/>
-      <c r="C98" s="29"/>
+      <c r="A98" s="22"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="23"/>
-      <c r="B99" s="23"/>
-      <c r="C99" s="23"/>
-    </row>
-    <row r="101" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="23"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+    </row>
+    <row r="102" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
+    <cfRule type="expression" dxfId="59" priority="60" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B24 A26:B35">
+    <cfRule type="expression" dxfId="58" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:B31">
+    <cfRule type="expression" dxfId="57" priority="58" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C39 C43:C46 C41">
+    <cfRule type="expression" dxfId="56" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B55 A58:B58">
+    <cfRule type="expression" dxfId="54" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C31">
+    <cfRule type="expression" dxfId="53" priority="55" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C55 C58">
+    <cfRule type="expression" dxfId="52" priority="48" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C39 C41">
+    <cfRule type="expression" dxfId="51" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C24 C26:C35">
+    <cfRule type="expression" dxfId="50" priority="56" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C53">
+    <cfRule type="expression" dxfId="49" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
+    <cfRule type="expression" dxfId="48" priority="54" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A41:B41">
+    <cfRule type="expression" dxfId="47" priority="53" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B53">
+    <cfRule type="expression" dxfId="46" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60 C62 C64:C65">
+    <cfRule type="expression" dxfId="45" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60 C62 C64:C69">
+    <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60 A62:B62 A64:B69">
+    <cfRule type="expression" dxfId="43" priority="46" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60 A62:B62 A64:B65">
+    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:B80">
+    <cfRule type="expression" dxfId="41" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:B76">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C76">
+    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C80">
+    <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B91">
+    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C87">
+    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C91">
+    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B87">
+    <cfRule type="expression" dxfId="33" priority="37" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
     <cfRule type="expression" dxfId="30" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="0" priority="30" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="28" priority="23" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
+  <conditionalFormatting sqref="A81">
+    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
     <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="26" priority="21" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C31">
+  <conditionalFormatting sqref="A37:B37">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
     <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="23" priority="22" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="21" priority="18" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="20" priority="25" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A70:B75">
+  <conditionalFormatting sqref="B37">
+    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:B42">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:B40">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
     <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81:B90">
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
     <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81:B86">
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
     <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="B58">
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
+  <conditionalFormatting sqref="A63:B63">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+  <conditionalFormatting sqref="C63">
     <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A80">
+  <conditionalFormatting sqref="C63">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add logs and meeting minutes
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0BF211-1C71-42E2-9A4C-BB7AF3C06B39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A831F6BF-0991-4371-9C22-A56A9B1BBAB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
     <sheet name="Week 2" sheetId="11" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$D$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$D$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$D$69</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="111">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -301,13 +303,64 @@
     <t>Dealing with python environment issues</t>
   </si>
   <si>
-    <t>IncluxDB Streaming</t>
-  </si>
-  <si>
     <t>Work on weekly presentation</t>
   </si>
   <si>
     <t>Upload OneDrive documents to GitHub with updated logs</t>
+  </si>
+  <si>
+    <t>Client slack discussions on the parser and meetings Monday</t>
+  </si>
+  <si>
+    <t>Testing how to query from InfluxDB for model training</t>
+  </si>
+  <si>
+    <t>Build derivative docker image for Telegraf with Python installed</t>
+  </si>
+  <si>
+    <t>InfluxDB Queries</t>
+  </si>
+  <si>
+    <t>Test continuous Python script call from Telegraf</t>
+  </si>
+  <si>
+    <t>Purging tokens from Github</t>
+  </si>
+  <si>
+    <t>InfluxDB Streaming Framework</t>
+  </si>
+  <si>
+    <t>Discuss EDA with Ryan</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>Setup meeting minutes for client meeting today and update Clubhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Management </t>
+  </si>
+  <si>
+    <t>Meeting with UDL on anomaly detection and streaming methods</t>
+  </si>
+  <si>
+    <t>Post client meeting to discuss direction</t>
+  </si>
+  <si>
+    <t>Correspondance with UDL on Friday meeting with Technical Safety BC</t>
+  </si>
+  <si>
+    <t>Project Communication</t>
+  </si>
+  <si>
+    <t>Building code to query InfluxDB records with detection model</t>
+  </si>
+  <si>
+    <t>Building code to write to InfluxDB records for detection model</t>
+  </si>
+  <si>
+    <t>Adding code to github after tokens purged from repo</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1166,483 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="159">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2129,7 +2658,7 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A82" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
@@ -2959,157 +3488,157 @@
     <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="90" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="89" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="88" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="87" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="86" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="85" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="84" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="83" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="82" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="81" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="80" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="79" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="78" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="77" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="76" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="75" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="74" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="73" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="72" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="71" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="70" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="69" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="68" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="67" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="66" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="65" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="63" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="62" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="61" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="60" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3127,8 +3656,8 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView showGridLines="0" topLeftCell="A85" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -3679,26 +4208,26 @@
         <v>64</v>
       </c>
       <c r="C60" s="25">
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="18" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C61" s="25">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C62" s="25">
         <v>0.25</v>
@@ -3706,46 +4235,46 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B63" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C63" s="25">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="C64" s="25">
-        <v>0.5</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B65" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C65" s="25">
-        <v>2.75</v>
+      <c r="B65" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="26">
+        <v>0.75</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="26">
-        <v>0.5</v>
+      <c r="C66" s="27">
+        <v>0.25</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -3764,7 +4293,7 @@
       <c r="C69" s="27"/>
       <c r="D69">
         <f>SUM(C60:C69)</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3838,24 +4367,48 @@
       <c r="C81" s="31"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="18"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
+      <c r="A82" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="18"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
+      <c r="A83" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="18"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
+      <c r="A84" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" s="18"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
+      <c r="A85" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="18"/>
@@ -3888,7 +4441,7 @@
       <c r="C91" s="27"/>
       <c r="D91">
         <f>SUM(C82:C91)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
@@ -3909,7 +4462,7 @@
       <c r="B94" s="17"/>
       <c r="C94" s="32">
         <f>SUM(C14:C91)</f>
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D94" s="13"/>
     </row>
@@ -3962,301 +4515,1327 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="59" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="58" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="57" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
+    <cfRule type="expression" dxfId="124" priority="56" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="expression" dxfId="123" priority="61" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B55 A58:B58">
+    <cfRule type="expression" dxfId="122" priority="54" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C31">
+    <cfRule type="expression" dxfId="121" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C55 C58">
+    <cfRule type="expression" dxfId="120" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C39 C41">
+    <cfRule type="expression" dxfId="119" priority="55" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C24 C26:C35">
+    <cfRule type="expression" dxfId="118" priority="60" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C53">
+    <cfRule type="expression" dxfId="117" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
+    <cfRule type="expression" dxfId="116" priority="58" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A41:B41">
+    <cfRule type="expression" dxfId="115" priority="57" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B53">
+    <cfRule type="expression" dxfId="114" priority="53" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C65">
+    <cfRule type="expression" dxfId="113" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C69">
+    <cfRule type="expression" dxfId="112" priority="48" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B69">
+    <cfRule type="expression" dxfId="111" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B65">
+    <cfRule type="expression" dxfId="110" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:B80">
+    <cfRule type="expression" dxfId="109" priority="46" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:B76">
+    <cfRule type="expression" dxfId="108" priority="45" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C76">
+    <cfRule type="expression" dxfId="107" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C80">
+    <cfRule type="expression" dxfId="106" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="105" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B91">
+    <cfRule type="expression" dxfId="104" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C87">
+    <cfRule type="expression" dxfId="103" priority="39" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C91">
+    <cfRule type="expression" dxfId="102" priority="40" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B87">
+    <cfRule type="expression" dxfId="101" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="100" priority="38" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="99" priority="37" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="expression" dxfId="98" priority="35" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="expression" dxfId="97" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="96" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="expression" dxfId="95" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B37">
+    <cfRule type="expression" dxfId="94" priority="31" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="expression" dxfId="93" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="expression" dxfId="92" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="91" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="expression" dxfId="90" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:B42">
+    <cfRule type="expression" dxfId="89" priority="26" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="expression" dxfId="88" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="87" priority="24" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="86" priority="23" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="85" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:B40">
+    <cfRule type="expression" dxfId="84" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="83" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="82" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="81" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="80" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="79" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="78" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="expression" dxfId="77" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="76" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="75" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="74" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="73" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="72" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="71" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="70" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="69" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="68" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="67" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="65" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="64" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.25"/>
+  <pageSetup scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81248D34-B6B9-4854-8289-D78F604F7C46}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D102"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="2">
+        <v>44333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="36">
+        <f>D3</f>
+        <v>44333</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="27">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="27">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="27">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="27">
+        <v>2.25</v>
+      </c>
+      <c r="D24">
+        <f>SUM(C15:C24)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="36">
+        <f>A14+1</f>
+        <v>44334</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="18"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="18"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="18"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="18"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="18"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="18"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="20"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="20"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="20"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35">
+        <f>SUM(C26:C35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="36">
+        <f>A25+1</f>
+        <v>44335</v>
+      </c>
+      <c r="B36" s="37"/>
+      <c r="C36" s="31"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="18"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="18"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="18"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="18"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="18"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="33"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="18"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="19"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="33"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="20"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="20"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46">
+        <f>SUM(C37:C46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="36">
+        <f>A36+1</f>
+        <v>44336</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="31"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="18"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="18"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="18"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="18"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="18"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="18"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="19"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="19"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="25"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="26"/>
+    </row>
+    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="35"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="34"/>
+      <c r="D58">
+        <f>SUM(C48:C58)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="36">
+        <f>A47+1</f>
+        <v>44337</v>
+      </c>
+      <c r="B59" s="37"/>
+      <c r="C59" s="31"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="18"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="18"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="18"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="18"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="18"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="19"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="20"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="20"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="20"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+    </row>
+    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="20"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69">
+        <f>SUM(C60:C69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="36">
+        <f>A59+1</f>
+        <v>44338</v>
+      </c>
+      <c r="B70" s="37"/>
+      <c r="C70" s="31"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="18"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="18"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="18"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="18"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="18"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="18"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="19"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="20"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="20"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+    </row>
+    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="20"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
+      <c r="D80">
+        <f>SUM(C71:C80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="36">
+        <f>A70+1</f>
+        <v>44339</v>
+      </c>
+      <c r="B81" s="37"/>
+      <c r="C81" s="31"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="18"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" s="18"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" s="18"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="25"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" s="18"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="25"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" s="18"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" s="18"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" s="19"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="20"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="27"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" s="20"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="20"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91">
+        <f>SUM(C82:C91)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="10"/>
+      <c r="B93" s="28"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="12"/>
+    </row>
+    <row r="94" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="17"/>
+      <c r="C94" s="32">
+        <f>SUM(C14:C91)</f>
+        <v>10</v>
+      </c>
+      <c r="D94" s="13"/>
+    </row>
+    <row r="95" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="9"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+    </row>
+    <row r="96" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A96" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="11"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="22"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="22"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="9"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="23"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+    </row>
+    <row r="102" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A70:B70"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="expression" dxfId="63" priority="64" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B24 A26:B35">
+    <cfRule type="expression" dxfId="62" priority="63" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:B31">
+    <cfRule type="expression" dxfId="61" priority="62" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C39 C43:C46 C41">
+    <cfRule type="expression" dxfId="60" priority="56" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="expression" dxfId="59" priority="61" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B55 A58:B58">
+    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C31">
+    <cfRule type="expression" dxfId="57" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C55 C58">
     <cfRule type="expression" dxfId="56" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="54" priority="50" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="53" priority="55" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="52" priority="48" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="51" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="50" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
+    <cfRule type="expression" dxfId="53" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
+    <cfRule type="expression" dxfId="52" priority="58" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A41:B41">
+    <cfRule type="expression" dxfId="51" priority="57" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B53">
+    <cfRule type="expression" dxfId="50" priority="53" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C65">
     <cfRule type="expression" dxfId="49" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="48" priority="54" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="47" priority="53" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B53">
+  <conditionalFormatting sqref="C60:C69">
+    <cfRule type="expression" dxfId="48" priority="48" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B69">
+    <cfRule type="expression" dxfId="47" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B65">
     <cfRule type="expression" dxfId="46" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60 C62 C64:C65">
-    <cfRule type="expression" dxfId="45" priority="43" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60 C62 C64:C69">
-    <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B60 A62:B62 A64:B69">
-    <cfRule type="expression" dxfId="43" priority="46" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B60 A62:B62 A64:B65">
-    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="41" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
+    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C80">
+    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="41" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B91">
+    <cfRule type="expression" dxfId="40" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C87">
     <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C80">
+  <conditionalFormatting sqref="C82:C91">
     <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B91">
+  <conditionalFormatting sqref="A82:B87">
+    <cfRule type="expression" dxfId="37" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
     <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="33" priority="37" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
+    <cfRule type="expression" dxfId="34" priority="35" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B37">
     <cfRule type="expression" dxfId="30" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
+  <conditionalFormatting sqref="A37">
     <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+  <conditionalFormatting sqref="B37">
     <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B37">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A42:B42">
     <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+  <conditionalFormatting sqref="A42">
     <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="B42">
     <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C40">
     <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42:B42">
+  <conditionalFormatting sqref="C40">
     <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+  <conditionalFormatting sqref="A40:B40">
     <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+  <conditionalFormatting sqref="A40">
     <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="B40">
     <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="A56:B57">
     <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:B40">
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
     <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
     <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
     <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+  <conditionalFormatting sqref="C62">
     <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+  <conditionalFormatting sqref="C62">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
+  <conditionalFormatting sqref="A62:B62">
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
update README and logs
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A831F6BF-0991-4371-9C22-A56A9B1BBAB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178F82E5-13EB-4CB1-AD1C-A0FFAC95BBA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -361,6 +361,48 @@
   </si>
   <si>
     <t>Adding code to github after tokens purged from repo</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Going through repo and update all code to use environment variables for tokens</t>
+  </si>
+  <si>
+    <t>Internal Meetings / Code Review</t>
+  </si>
+  <si>
+    <t>Stand-up / discussion on PR / go over presentation</t>
+  </si>
+  <si>
+    <t>UBC Prof Meeting</t>
+  </si>
+  <si>
+    <t>UBC Meeting</t>
+  </si>
+  <si>
+    <t>Anomaly Detection Research</t>
+  </si>
+  <si>
+    <t>Parsing InfluxDB line protocol for predict method</t>
+  </si>
+  <si>
+    <t>Discuss anomaly detection algorithms and read paper</t>
+  </si>
+  <si>
+    <t>Extended stand-up discussion plan/project schedule</t>
+  </si>
+  <si>
+    <t>PR streaming framework code (putting it on hold for now)</t>
+  </si>
+  <si>
+    <t>Update docker files related to testing the InfluxDB streaming setup</t>
+  </si>
+  <si>
+    <t>Sprint planning doc prep and Clubhouse prep/clean-up</t>
+  </si>
+  <si>
+    <t>Work on week 4 status presentation</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1208,42 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="159">
+  <dxfs count="164">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3488,157 +3565,157 @@
     <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="158" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="157" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="156" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="155" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="154" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="153" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="152" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="151" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="150" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="149" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="148" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="147" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="146" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="145" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="144" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="143" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="142" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="141" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="140" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="139" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="138" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="137" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="136" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="135" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="134" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="133" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="132" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="131" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="130" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="129" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="128" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3656,7 +3733,7 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A85" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
@@ -4515,322 +4592,322 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="127" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="126" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="125" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="124" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="123" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="122" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="121" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="120" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="119" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="118" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="117" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="116" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="115" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="114" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="113" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="112" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="111" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="110" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="109" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="108" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="107" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="106" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="105" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="104" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="103" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="102" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="101" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="100" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="99" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="98" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="97" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="96" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="95" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="94" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="93" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="92" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="91" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="90" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="89" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="88" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="87" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="86" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="85" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B40">
-    <cfRule type="expression" dxfId="84" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="83" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="82" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="81" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="80" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="79" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="78" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="77" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="76" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="75" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="74" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="73" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="72" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="71" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="70" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="69" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="68" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="67" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="65" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="64" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4848,8 +4925,8 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -5078,41 +5155,77 @@
         <v>110</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C26" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="18"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="18"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="18"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="18"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
+      <c r="A32" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="26">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="20"/>
@@ -5130,7 +5243,7 @@
       <c r="C35" s="27"/>
       <c r="D35">
         <f>SUM(C26:C35)</f>
-        <v>1</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5142,35 +5255,71 @@
       <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="18"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="18"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="18"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+      <c r="A41" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="25">
+        <v>1</v>
+      </c>
       <c r="D41" s="33"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="18"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="19"/>
@@ -5194,7 +5343,7 @@
       <c r="C46" s="27"/>
       <c r="D46">
         <f>SUM(C37:C46)</f>
-        <v>0</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5468,7 +5617,7 @@
       <c r="B94" s="17"/>
       <c r="C94" s="32">
         <f>SUM(C14:C91)</f>
-        <v>10</v>
+        <v>25.75</v>
       </c>
       <c r="D94" s="13"/>
     </row>
@@ -5521,322 +5670,347 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="63" priority="64" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="62" priority="63" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="61" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="70" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B24 A26:B29 A31:B35">
+    <cfRule type="expression" dxfId="67" priority="69" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:B29 A31:B31">
+    <cfRule type="expression" dxfId="66" priority="68" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="60" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="59" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="67" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="57" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="60" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C29 C31">
+    <cfRule type="expression" dxfId="62" priority="65" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="56" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="55" priority="55" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="54" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="61" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C24 C26:C29 C31:C35">
+    <cfRule type="expression" dxfId="59" priority="66" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="53" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="52" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="51" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="50" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="49" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="48" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
+    <cfRule type="expression" dxfId="52" priority="56" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B65">
+    <cfRule type="expression" dxfId="51" priority="55" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:B80">
+    <cfRule type="expression" dxfId="50" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:B76">
+    <cfRule type="expression" dxfId="49" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C76">
+    <cfRule type="expression" dxfId="48" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C80">
     <cfRule type="expression" dxfId="47" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="46" priority="49" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A71:B76">
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="46" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B91">
+    <cfRule type="expression" dxfId="45" priority="48" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C87">
     <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="41" priority="36" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="40" priority="42" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
+    <cfRule type="expression" dxfId="43" priority="46" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B87">
+    <cfRule type="expression" dxfId="42" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="40" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="expression" dxfId="39" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
     <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="37" priority="41" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="37" priority="39" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
     <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
+  <conditionalFormatting sqref="A37:B37">
     <cfRule type="expression" dxfId="35" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="34" priority="35" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="30" priority="31" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="27" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
     <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40:B40">
-    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="22" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
     <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:B30">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:B30">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add dashboard research and update logs
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178F82E5-13EB-4CB1-AD1C-A0FFAC95BBA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FF1837-4E90-4404-827A-D6F8BB5A7F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="136">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -403,6 +403,39 @@
   </si>
   <si>
     <t>Work on week 4 status presentation</t>
+  </si>
+  <si>
+    <t>Update logs and github</t>
+  </si>
+  <si>
+    <t>Review anomaly detection research PR</t>
+  </si>
+  <si>
+    <t>Presentation for Tech Safety BC meeting Friday</t>
+  </si>
+  <si>
+    <t>Project Documents/Client Meetings</t>
+  </si>
+  <si>
+    <t>Review EDA PR</t>
+  </si>
+  <si>
+    <t>Dashboard Research</t>
+  </si>
+  <si>
+    <t>Initial research on Grafana to understand dashboard level-of-effort</t>
+  </si>
+  <si>
+    <t>Helping UDL with data streaming parsing</t>
+  </si>
+  <si>
+    <t>Streaming Parsing support for UDL</t>
+  </si>
+  <si>
+    <t>Document Grafana research (sufficient understanding for now)</t>
+  </si>
+  <si>
+    <t>Discuss anomaly detection approach w/ Ryan and generate schematic</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1241,21 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="164">
+  <dxfs count="166">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2735,7 +2782,7 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A82" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
@@ -3565,157 +3612,157 @@
     <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="163" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="162" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="161" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="160" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="159" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="158" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="157" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="156" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="155" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="154" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="153" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="152" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="151" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="150" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="149" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="148" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="147" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="146" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="145" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="144" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="143" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="142" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="141" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="140" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="139" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="138" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="137" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="136" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="135" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="134" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="133" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3733,7 +3780,7 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
@@ -4592,322 +4639,322 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="132" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="131" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="130" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="129" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="128" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="127" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="126" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="125" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="124" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="123" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="122" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="121" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="120" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="119" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="118" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="117" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="116" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="115" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="114" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="113" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="112" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="111" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="110" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="109" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="108" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="106" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="105" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="104" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="103" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="102" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="101" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="100" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="99" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="98" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="97" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="96" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="95" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="94" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="93" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="92" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="91" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="90" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B40">
-    <cfRule type="expression" dxfId="89" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="88" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="87" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="86" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="85" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="84" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="83" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="82" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="81" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="79" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="78" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="77" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="76" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="75" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="74" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="73" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="72" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="71" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="70" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="69" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4925,8 +4972,8 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -5322,28 +5369,52 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="19"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="26">
+        <v>0.25</v>
+      </c>
       <c r="D43" s="33"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="20"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="20"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="27">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="20"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="27">
+        <v>0.5</v>
+      </c>
       <c r="D46">
         <f>SUM(C37:C46)</f>
-        <v>7.25</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5355,34 +5426,70 @@
       <c r="C47" s="31"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="18"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
+      <c r="A48" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="18"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="A49" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="18"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="25">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="18"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="25">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="25">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="19"/>
@@ -5410,7 +5517,7 @@
       <c r="C58" s="34"/>
       <c r="D58">
         <f>SUM(C48:C58)</f>
-        <v>0</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5617,7 +5724,7 @@
       <c r="B94" s="17"/>
       <c r="C94" s="32">
         <f>SUM(C14:C91)</f>
-        <v>25.75</v>
+        <v>38.25</v>
       </c>
       <c r="D94" s="13"/>
     </row>
@@ -5670,346 +5777,356 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
+    <cfRule type="expression" dxfId="70" priority="72" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B24 A26:B29 A31:B35">
+    <cfRule type="expression" dxfId="69" priority="71" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:B29 A31:B31">
     <cfRule type="expression" dxfId="68" priority="70" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:B24 A26:B29 A31:B35">
-    <cfRule type="expression" dxfId="67" priority="69" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:B29 A31:B31">
-    <cfRule type="expression" dxfId="66" priority="68" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
+    <cfRule type="expression" dxfId="67" priority="64" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="expression" dxfId="66" priority="69" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B55 A58:B58">
     <cfRule type="expression" dxfId="65" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
+  <conditionalFormatting sqref="C26:C29 C31">
     <cfRule type="expression" dxfId="64" priority="67" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B55 A58:B58">
+  <conditionalFormatting sqref="C48:C55 C58">
     <cfRule type="expression" dxfId="63" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C29 C31">
-    <cfRule type="expression" dxfId="62" priority="65" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="61" priority="58" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="60" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C29 C31:C35">
+    <cfRule type="expression" dxfId="61" priority="68" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C53">
+    <cfRule type="expression" dxfId="60" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39 A43:B43 A41:B41 A45:B46 A44">
     <cfRule type="expression" dxfId="59" priority="66" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="58" priority="57" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="57" priority="64" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="56" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="65" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="55" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="54" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="53" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="52" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="51" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="50" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="49" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="48" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
+    <cfRule type="expression" dxfId="49" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="48" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:B91">
     <cfRule type="expression" dxfId="47" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="46" priority="42" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B91">
+  <conditionalFormatting sqref="C82:C87">
+    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C91">
     <cfRule type="expression" dxfId="45" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C91">
+  <conditionalFormatting sqref="A82:B87">
+    <cfRule type="expression" dxfId="44" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
     <cfRule type="expression" dxfId="43" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="42" priority="47" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="40" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
+    <cfRule type="expression" dxfId="41" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="expression" dxfId="40" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
     <cfRule type="expression" dxfId="39" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
+  <conditionalFormatting sqref="B32">
     <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+  <conditionalFormatting sqref="A37:B37">
     <cfRule type="expression" dxfId="37" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
+  <conditionalFormatting sqref="A37">
     <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B37">
+  <conditionalFormatting sqref="B37">
     <cfRule type="expression" dxfId="35" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="33" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="A42:B42">
     <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="A42">
     <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42:B42">
+  <conditionalFormatting sqref="B42">
     <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
+  <conditionalFormatting sqref="C40">
     <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+  <conditionalFormatting sqref="C40">
     <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="A40">
     <cfRule type="expression" dxfId="27" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="A40">
     <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="22" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
+  <conditionalFormatting sqref="B44">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
update logs and weekly ptt
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FF1837-4E90-4404-827A-D6F8BB5A7F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBFEFC9-6188-46C7-8360-14F2467D43B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="151">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -436,6 +436,51 @@
   </si>
   <si>
     <t>Discuss anomaly detection approach w/ Ryan and generate schematic</t>
+  </si>
+  <si>
+    <t>Update PowerPoint for meeting with TechSafety BC</t>
+  </si>
+  <si>
+    <t>Anomaly Detection Model</t>
+  </si>
+  <si>
+    <t>Anomaly detection model discussions</t>
+  </si>
+  <si>
+    <t>Meeting with TechSafetyBC</t>
+  </si>
+  <si>
+    <t>Post meeting discussion with UDL and discussionon next steps</t>
+  </si>
+  <si>
+    <t>Client Meetings / Data Access</t>
+  </si>
+  <si>
+    <t>Go over with Ryan how to start downloading data from SkySpark manually</t>
+  </si>
+  <si>
+    <t>Data Access</t>
+  </si>
+  <si>
+    <t>Meeting with Scott to discuss proposed method</t>
+  </si>
+  <si>
+    <t>Post meeting discussion</t>
+  </si>
+  <si>
+    <t>Internal Meeting</t>
+  </si>
+  <si>
+    <t>Figuring out a way to easily view and label anomalies</t>
+  </si>
+  <si>
+    <t>Anomaly Labelling</t>
+  </si>
+  <si>
+    <t>Built a Shiny app to support labelling anomalies</t>
+  </si>
+  <si>
+    <t>Update Week 4 Status Presentation</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1286,28 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="166">
+  <dxfs count="169">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2782,7 +2848,7 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
@@ -3612,157 +3678,157 @@
     <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="165" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="164" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="163" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="162" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="161" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="160" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="159" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="158" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="157" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="156" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="155" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="154" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="153" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="152" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="151" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="150" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="149" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="148" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="147" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="146" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="145" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="144" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="143" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="142" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="141" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="140" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="139" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="138" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="137" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="136" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="135" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3780,7 +3846,7 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A55" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
@@ -4639,322 +4705,322 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="134" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="133" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="132" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="131" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="130" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="129" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="128" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="127" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="126" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="125" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="124" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="123" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="122" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="121" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="120" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="119" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="118" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="117" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="116" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="115" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="114" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="113" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="112" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="111" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="110" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="109" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="108" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="107" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="106" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="105" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="104" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="103" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="102" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="101" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="100" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="99" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="98" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="97" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="96" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="95" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="94" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="93" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="92" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B40">
-    <cfRule type="expression" dxfId="91" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="90" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="89" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="88" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="87" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="86" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="85" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="84" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="83" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="82" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="81" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="80" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="79" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="78" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="77" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="76" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="75" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="74" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="73" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="72" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="71" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4973,7 +5039,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -5492,9 +5558,15 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="19"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
+      <c r="A54" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="19"/>
@@ -5517,7 +5589,7 @@
       <c r="C58" s="34"/>
       <c r="D58">
         <f>SUM(C48:C58)</f>
-        <v>9.25</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5529,44 +5601,92 @@
       <c r="C59" s="31"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="18"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
+      <c r="A62" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="18"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
+      <c r="A63" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="25">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="18"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
+      <c r="A64" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="19"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
+      <c r="A65" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="26">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="20"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="27">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="20"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="27">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="20"/>
@@ -5579,7 +5699,7 @@
       <c r="C69" s="27"/>
       <c r="D69">
         <f>SUM(C60:C69)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5591,14 +5711,26 @@
       <c r="C70" s="31"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
+      <c r="A71" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="25">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="18"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
+      <c r="A72" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="18"/>
@@ -5641,7 +5773,7 @@
       <c r="C80" s="27"/>
       <c r="D80">
         <f>SUM(C71:C80)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5724,7 +5856,7 @@
       <c r="B94" s="17"/>
       <c r="C94" s="32">
         <f>SUM(C14:C91)</f>
-        <v>38.25</v>
+        <v>57.75</v>
       </c>
       <c r="D94" s="13"/>
     </row>
@@ -5777,357 +5909,372 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="70" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="76" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B29 A31:B35">
-    <cfRule type="expression" dxfId="69" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="75" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B29 A31:B31">
-    <cfRule type="expression" dxfId="68" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="74" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="67" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="68" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="66" priority="69" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="65" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="73" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:B53 A58:B58 A55:B55">
+    <cfRule type="expression" dxfId="68" priority="66" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C29 C31">
-    <cfRule type="expression" dxfId="64" priority="67" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="63" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="71" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C53 C58 C55">
+    <cfRule type="expression" dxfId="66" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="62" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="67" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C29 C31:C35">
-    <cfRule type="expression" dxfId="61" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="72" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="60" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B43 A41:B41 A45:B46 A44">
-    <cfRule type="expression" dxfId="59" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="70" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="58" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="57" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="65" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="56" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="55" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="53" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="52" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="51" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="50" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="49" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="48" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="47" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="45" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="44" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="46" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="45" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70">
+    <cfRule type="expression" dxfId="44" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
     <cfRule type="expression" dxfId="43" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
+  <conditionalFormatting sqref="A32">
     <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="41" priority="43" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="40" priority="42" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="39" priority="41" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="37" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="35" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="33" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="31" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="29" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
     <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="27" priority="29" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="22" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
     <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
     <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
     <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+  <conditionalFormatting sqref="C62">
     <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+  <conditionalFormatting sqref="C62">
     <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
+  <conditionalFormatting sqref="A62:B62">
     <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
+  <conditionalFormatting sqref="A30:B30">
     <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
+  <conditionalFormatting sqref="A30:B30">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
     <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30:B30">
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
     <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:B30">
+  <conditionalFormatting sqref="B40">
     <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B54">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B54">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update logs add meeting docs
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBFEFC9-6188-46C7-8360-14F2467D43B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3865EC-4415-493A-A079-511F8BDD753A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="152">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>Update Week 4 Status Presentation</t>
+  </si>
+  <si>
+    <t>Anomaly labelling</t>
   </si>
 </sst>
 </file>
@@ -5038,8 +5041,8 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -5785,9 +5788,15 @@
       <c r="C81" s="31"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="18"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
+      <c r="A82" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="25">
+        <v>7</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="18"/>
@@ -5835,7 +5844,7 @@
       <c r="C91" s="27"/>
       <c r="D91">
         <f>SUM(C82:C91)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
@@ -5856,7 +5865,7 @@
       <c r="B94" s="17"/>
       <c r="C94" s="32">
         <f>SUM(C14:C91)</f>
-        <v>57.75</v>
+        <v>64.75</v>
       </c>
       <c r="D94" s="13"/>
     </row>

</xml_diff>

<commit_message>
update logs and README
</commit_message>
<xml_diff>
--- a/personal-logs/nathan-smith/WorkLog_ns.xlsx
+++ b/personal-logs/nathan-smith/WorkLog_ns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B52A4AD-A32D-4F27-B427-0C8FAA34F36D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D259CEB-B223-4AAD-8BCA-6A03FDDEAB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="203">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -606,6 +606,39 @@
   </si>
   <si>
     <t>Code discussion with Ryan</t>
+  </si>
+  <si>
+    <t>Commit various project management docs to github and setup minutes for Monday</t>
+  </si>
+  <si>
+    <t>PR review on model pipeline</t>
+  </si>
+  <si>
+    <t>Discuss spectral residual transformation with Debangsha</t>
+  </si>
+  <si>
+    <t>Final Report</t>
+  </si>
+  <si>
+    <t>Start report template (waiting on code) and discuss report with Ryan</t>
+  </si>
+  <si>
+    <t>Custom transformer class for spectral residual code</t>
+  </si>
+  <si>
+    <t>Discuss preliminary model results and results template notebook</t>
+  </si>
+  <si>
+    <t>Model Results</t>
+  </si>
+  <si>
+    <t>Modelling</t>
+  </si>
+  <si>
+    <t>Researching various LSTM architectures</t>
+  </si>
+  <si>
+    <t>Researching various LSTM architectures (incl discussion with Ryan)</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1461,49 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="252">
+  <dxfs count="258">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4401,157 +4476,157 @@
     <mergeCell ref="A69:B69"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="251" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="257" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="250" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="256" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="249" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="255" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="248" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="254" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="247" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="253" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B57">
-    <cfRule type="expression" dxfId="246" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="252" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="245" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="251" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="244" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="250" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="243" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="249" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="242" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="248" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="241" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="247" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="240" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="246" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="239" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="245" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="238" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="244" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="237" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="243" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="236" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="242" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="235" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="241" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="234" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="240" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="233" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="239" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="232" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="238" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="231" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="237" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="230" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="236" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="229" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="235" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B90">
-    <cfRule type="expression" dxfId="228" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="234" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C86">
-    <cfRule type="expression" dxfId="227" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="233" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:C90">
-    <cfRule type="expression" dxfId="226" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="232" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81:B86">
-    <cfRule type="expression" dxfId="225" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="231" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="224" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="230" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="223" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="229" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="222" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="228" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80">
-    <cfRule type="expression" dxfId="221" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="227" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5428,322 +5503,322 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="220" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="226" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B35">
-    <cfRule type="expression" dxfId="219" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="225" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B31">
-    <cfRule type="expression" dxfId="218" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="224" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="217" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="223" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="216" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="222" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B55 A58:B58">
-    <cfRule type="expression" dxfId="215" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="221" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C31">
-    <cfRule type="expression" dxfId="214" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C55 C58">
-    <cfRule type="expression" dxfId="213" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="219" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="212" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="218" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C35">
-    <cfRule type="expression" dxfId="211" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="217" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="210" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B46 A41:B41">
-    <cfRule type="expression" dxfId="209" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="208" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="207" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="206" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="205" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="204" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="203" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="202" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="201" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="200" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="199" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="205" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="198" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="197" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="196" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="195" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="194" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="193" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="192" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="191" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="197" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="190" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="189" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="188" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="187" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="186" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="185" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="191" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="184" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="183" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="182" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="181" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="180" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="179" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="178" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B40">
-    <cfRule type="expression" dxfId="177" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="176" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="175" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="174" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="173" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="172" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="171" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" dxfId="170" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="169" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="168" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="167" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="166" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="165" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="164" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="163" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="162" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="161" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="160" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="159" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="158" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="157" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6638,372 +6713,372 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="156" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="76" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B24 A26:B29 A31:B35">
-    <cfRule type="expression" dxfId="155" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="75" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B29 A31:B31">
-    <cfRule type="expression" dxfId="154" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="74" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="153" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="68" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="152" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="73" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53 A58:B58 A55:B55">
-    <cfRule type="expression" dxfId="151" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="66" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C29 C31">
-    <cfRule type="expression" dxfId="150" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53 C58 C55">
-    <cfRule type="expression" dxfId="149" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="148" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="67" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C29 C31:C35">
-    <cfRule type="expression" dxfId="147" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="72" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="146" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A43:B43 A41:B41 A45:B46 A44">
-    <cfRule type="expression" dxfId="145" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="70" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39 A41:B41">
-    <cfRule type="expression" dxfId="144" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="69" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="143" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="65" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="142" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="141" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="140" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="139" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="138" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="137" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="136" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
-    <cfRule type="expression" dxfId="135" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="134" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="48" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="133" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="132" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="131" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="130" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="129" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="128" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="expression" dxfId="127" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="47" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A81">
-    <cfRule type="expression" dxfId="126" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="125" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="124" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="123" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="122" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="121" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="120" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="119" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="118" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="117" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="116" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="115" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="114" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="113" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="112" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="111" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="110" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="109" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="108" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="107" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="106" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="105" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="104" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="103" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="102" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="101" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="100" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="99" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="98" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="97" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="96" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="95" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="94" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="93" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="92" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="91" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="90" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="89" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="88" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="87" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:B54">
-    <cfRule type="expression" dxfId="86" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="85" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="84" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:B54">
-    <cfRule type="expression" dxfId="83" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7021,8 +7096,8 @@
   </sheetPr>
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -7585,50 +7660,104 @@
       <c r="B59" s="42"/>
       <c r="C59" s="31"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.35">
+      <c r="A60" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="18"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
+      <c r="A62" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="18"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
+      <c r="A63" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="18"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
+      <c r="A64" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="19"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
+      <c r="A65" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="26">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="20"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="C66" s="27">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="20"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" s="27">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="20"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
+      <c r="A68" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" s="27">
+        <v>3</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="20"/>
@@ -7636,7 +7765,7 @@
       <c r="C69" s="27"/>
       <c r="D69">
         <f>SUM(C60:C69)</f>
-        <v>0</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7648,14 +7777,26 @@
       <c r="C70" s="31"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
+      <c r="A71" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" s="18"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
+      <c r="A72" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B72" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" s="25">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="18"/>
@@ -7698,7 +7839,7 @@
       <c r="C80" s="27"/>
       <c r="D80">
         <f>SUM(C71:C80)</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7710,9 +7851,15 @@
       <c r="C81" s="31"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="18"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
+      <c r="A82" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B82" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="18"/>
@@ -7760,7 +7907,7 @@
       <c r="C91" s="27"/>
       <c r="D91">
         <f>SUM(C82:C91)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
@@ -7781,7 +7928,7 @@
       <c r="B94" s="17"/>
       <c r="C94" s="32">
         <f>SUM(C14:C91)</f>
-        <v>33.5</v>
+        <v>54.75</v>
       </c>
       <c r="D94" s="13"/>
     </row>
@@ -7834,416 +7981,446 @@
     <mergeCell ref="A70:B70"/>
   </mergeCells>
   <conditionalFormatting sqref="A14">
-    <cfRule type="expression" dxfId="82" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="92" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B29 A15:B24 A31:B35">
-    <cfRule type="expression" dxfId="81" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="91" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B29 A31:B31">
-    <cfRule type="expression" dxfId="80" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="90" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C43:C46 C41">
-    <cfRule type="expression" dxfId="79" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="84" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="78" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="89" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B58 A55:B55 A48:B53">
-    <cfRule type="expression" dxfId="77" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="82" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C29 C31">
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="87" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53 C58 C55">
-    <cfRule type="expression" dxfId="75" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="80" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C39 C41">
-    <cfRule type="expression" dxfId="74" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="83" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C24 C26:C29 C31:C35">
-    <cfRule type="expression" dxfId="73" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="88" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="72" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39 A43:B43 A41:B41 A46:B46 A38 A44:A45">
-    <cfRule type="expression" dxfId="71" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="86" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39 A41:B41 A38">
-    <cfRule type="expression" dxfId="70" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="85" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B53">
-    <cfRule type="expression" dxfId="69" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="81" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C65">
-    <cfRule type="expression" dxfId="68" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="75" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C69">
-    <cfRule type="expression" dxfId="67" priority="70" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B69">
-    <cfRule type="expression" dxfId="66" priority="72" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B65">
-    <cfRule type="expression" dxfId="65" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="76" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B64 A66:B69 A65">
+    <cfRule type="expression" dxfId="72" priority="78" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B64 A65">
+    <cfRule type="expression" dxfId="71" priority="77" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B80">
-    <cfRule type="expression" dxfId="64" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="74" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71:B76">
-    <cfRule type="expression" dxfId="63" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="73" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C76">
-    <cfRule type="expression" dxfId="62" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C80">
+    <cfRule type="expression" dxfId="67" priority="72" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="66" priority="64" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83:B91 B82">
+    <cfRule type="expression" dxfId="65" priority="70" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C87">
+    <cfRule type="expression" dxfId="64" priority="67" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C82:C91">
+    <cfRule type="expression" dxfId="63" priority="68" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A83:B87 B82">
+    <cfRule type="expression" dxfId="62" priority="69" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
     <cfRule type="expression" dxfId="61" priority="66" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="60" priority="58" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B91">
-    <cfRule type="expression" dxfId="59" priority="64" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C87">
-    <cfRule type="expression" dxfId="58" priority="61" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82:C91">
-    <cfRule type="expression" dxfId="57" priority="62" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A82:B87">
-    <cfRule type="expression" dxfId="56" priority="63" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="55" priority="60" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="65" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
+    <cfRule type="expression" dxfId="59" priority="63" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A81">
+    <cfRule type="expression" dxfId="58" priority="62" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="57" priority="61" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="expression" dxfId="56" priority="60" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B37">
+    <cfRule type="expression" dxfId="55" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
     <cfRule type="expression" dxfId="53" priority="57" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="52" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
+  <conditionalFormatting sqref="C42">
     <cfRule type="expression" dxfId="51" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A42:B42">
+    <cfRule type="expression" dxfId="50" priority="54" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="expression" dxfId="49" priority="53" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42">
+    <cfRule type="expression" dxfId="48" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="47" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="expression" dxfId="46" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="45" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="44" priority="48" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="43" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="42" priority="45" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56:C57">
+    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="40" priority="46" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="39" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="38" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="37" priority="40" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B61">
+    <cfRule type="expression" dxfId="36" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="35" priority="39" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="34" priority="38" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="33" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="31" priority="37" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="30" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="29" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="27" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:B30">
+    <cfRule type="expression" dxfId="26" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:B30">
+    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="24" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="23" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="expression" dxfId="17" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="50" priority="54" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="49" priority="53" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="48" priority="52" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="47" priority="51" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="46" priority="50" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="45" priority="49" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="44" priority="48" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="43" priority="47" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="42" priority="46" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="41" priority="45" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="40" priority="44" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="39" priority="43" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="38" priority="42" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="37" priority="41" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="36" priority="39" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56:C57">
-    <cfRule type="expression" dxfId="35" priority="38" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="34" priority="40" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="33" priority="37" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="31" priority="34" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="30" priority="36" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58">
-    <cfRule type="expression" dxfId="29" priority="33" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="27" priority="30" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="21" priority="27" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="17" priority="22" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="15" priority="19" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
     <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+  <conditionalFormatting sqref="B44">
     <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="expression" dxfId="11" priority="15" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
     <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
+  <conditionalFormatting sqref="B54">
     <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
+  <conditionalFormatting sqref="B54">
     <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
+  <conditionalFormatting sqref="B63">
     <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
+  <conditionalFormatting sqref="B63">
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
+  <conditionalFormatting sqref="B65">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
+  <conditionalFormatting sqref="B65">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
+  <conditionalFormatting sqref="A82">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
+  <conditionalFormatting sqref="A82">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>